<commit_message>
adjust results file to correct names of variables
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/Empirical_Study/empirical-study-dfds/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/empirical_study_DFDs/GitHub_replication_package/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F084814-D9C3-6042-95C1-A8E4F665D696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFE2D4A-5BDF-DD44-87B0-DA746A379C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" activeTab="1" xr2:uid="{E68C5B94-9B04-2047-B6F9-6FC8248CDF83}"/>
   </bookViews>
   <sheets>
-    <sheet name="With DFD" sheetId="1" r:id="rId1"/>
-    <sheet name="Without DFD" sheetId="2" r:id="rId2"/>
+    <sheet name="control condition" sheetId="2" r:id="rId1"/>
+    <sheet name="model-supported condition" sheetId="1" r:id="rId2"/>
     <sheet name="Questionnaire" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="130">
   <si>
     <t xml:space="preserve">How helpful was the provided architectural diagram (Dataflow Diagram) for performing the tasks? </t>
   </si>
@@ -374,68 +374,72 @@
     <t>0: None or could not answer</t>
   </si>
   <si>
-    <t>Task1_score</t>
-  </si>
-  <si>
-    <t>Task1_evidence</t>
-  </si>
-  <si>
     <t>Task1_resource</t>
   </si>
   <si>
     <t>arch</t>
   </si>
   <si>
-    <t>Task2_score</t>
-  </si>
-  <si>
-    <t>Task2_evidence</t>
-  </si>
-  <si>
     <t>Task2_resource</t>
   </si>
   <si>
-    <t>Task3_score</t>
-  </si>
-  <si>
-    <t>Task3_evidence</t>
-  </si>
-  <si>
     <t>Task3_resource</t>
   </si>
   <si>
-    <t>Task4_score</t>
-  </si>
-  <si>
-    <t>Task4_evidence</t>
-  </si>
-  <si>
     <t>Task4_resource</t>
   </si>
   <si>
-    <t>Task5_score</t>
-  </si>
-  <si>
-    <t>Task5_evidence</t>
-  </si>
-  <si>
     <t>Task5_resource</t>
   </si>
   <si>
-    <t>Task6_score</t>
-  </si>
-  <si>
-    <t>Task6_evidence</t>
-  </si>
-  <si>
     <t>Task6_resource</t>
+  </si>
+  <si>
+    <t>did not answer 
+correctly</t>
+  </si>
+  <si>
+    <t>Task1_analysis_correctness</t>
+  </si>
+  <si>
+    <t>Task2_analysis_correctness</t>
+  </si>
+  <si>
+    <t>Task3_analysis_correctness</t>
+  </si>
+  <si>
+    <t>Task4_analysis_correctness</t>
+  </si>
+  <si>
+    <t>Task5_analysis_correctness</t>
+  </si>
+  <si>
+    <t>Task6_analysis_correctness</t>
+  </si>
+  <si>
+    <t>Task1_correctness_of_evidence</t>
+  </si>
+  <si>
+    <t>Task2_correctness_of_evidence</t>
+  </si>
+  <si>
+    <t>Task3_correctness_of_evidence</t>
+  </si>
+  <si>
+    <t>Task4_correctness_of_evidence</t>
+  </si>
+  <si>
+    <t>Task5_correctness_of_evidence</t>
+  </si>
+  <si>
+    <t>Task6_correctness_of_evidence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -453,6 +457,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -586,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -664,22 +675,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -988,11 +991,1946 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5FF93F-B917-3747-9BBB-00B8CF48955D}">
+  <dimension ref="A1:AB31"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="15" width="13.83203125" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="21" max="21" width="12.5" customWidth="1"/>
+    <col min="22" max="22" width="57.1640625" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15">
+        <v>2</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="26">
+        <v>0</v>
+      </c>
+      <c r="I2" s="15">
+        <v>2</v>
+      </c>
+      <c r="J2" s="26">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="26">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="15">
+        <v>0</v>
+      </c>
+      <c r="P2" s="26">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="28">
+        <v>1</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="15">
+        <v>2</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="15">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="23">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="15">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="15">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1</v>
+      </c>
+      <c r="U4" s="9">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="23">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="15">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="15">
+        <v>2</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="15">
+        <v>2</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5" s="9">
+        <v>2</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="15">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="9">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15">
+        <v>2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="15">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="15">
+        <v>2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3">
+        <v>1</v>
+      </c>
+      <c r="U7" s="9">
+        <v>2</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="15">
+        <v>2</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="15">
+        <v>2</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="15">
+        <v>2</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="9">
+        <v>2</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>2</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="15">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="15">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="15">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="9">
+        <v>1</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="23">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>2</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="15">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="15">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="15">
+        <v>2</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1</v>
+      </c>
+      <c r="U10" s="9">
+        <v>1</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="23">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15">
+        <v>2</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="15">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="15">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="15">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11" s="15">
+        <v>2</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="9">
+        <v>2</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="23">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <v>2</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="15">
+        <v>1</v>
+      </c>
+      <c r="P12" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12" s="15">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>1</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0</v>
+      </c>
+      <c r="U12" s="9">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="23">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>2</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="15">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="15">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+      <c r="R13" s="15">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1">
+        <v>1</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0</v>
+      </c>
+      <c r="U13" s="9">
+        <v>1</v>
+      </c>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="15">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="15">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="15">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+      <c r="R14" s="15">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>1</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="U14" s="9">
+        <v>2</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W14" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="23">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+      <c r="R15" s="15">
+        <v>2</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="9">
+        <v>2</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="23">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="15">
+        <v>2</v>
+      </c>
+      <c r="G16" s="13">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
+      <c r="R16" s="15">
+        <v>2</v>
+      </c>
+      <c r="S16" s="1">
+        <v>1</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1</v>
+      </c>
+      <c r="U16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="23">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="15">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>2</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="15">
+        <v>2</v>
+      </c>
+      <c r="P17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="15">
+        <v>2</v>
+      </c>
+      <c r="S17" s="1">
+        <v>1</v>
+      </c>
+      <c r="T17" s="3">
+        <v>0</v>
+      </c>
+      <c r="U17" s="9">
+        <v>2</v>
+      </c>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="23">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="15">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="15">
+        <v>2</v>
+      </c>
+      <c r="P18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="15">
+        <v>2</v>
+      </c>
+      <c r="S18" s="1">
+        <v>1</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0</v>
+      </c>
+      <c r="U18" s="9">
+        <v>2</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W18" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
+        <v>2</v>
+      </c>
+      <c r="G19" s="13">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="15">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="15">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="15">
+        <v>2</v>
+      </c>
+      <c r="S19" s="1">
+        <v>1</v>
+      </c>
+      <c r="T19" s="3">
+        <v>0</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="23">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="15">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="15">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="15">
+        <v>2</v>
+      </c>
+      <c r="S20" s="1">
+        <v>1</v>
+      </c>
+      <c r="T20" s="3">
+        <v>0</v>
+      </c>
+      <c r="U20" s="9">
+        <v>2</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="23">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15">
+        <v>2</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="15">
+        <v>2</v>
+      </c>
+      <c r="M21" s="1">
+        <v>2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="15">
+        <v>2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="15">
+        <v>2</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="9">
+        <v>2</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23">
+        <v>47</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="15">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="15">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="15">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="15">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="9">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W22" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="23">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="15">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="15">
+        <v>2</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="15">
+        <v>2</v>
+      </c>
+      <c r="S23" s="1">
+        <v>1</v>
+      </c>
+      <c r="T23" s="3">
+        <v>1</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="23">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="15">
+        <v>2</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="15">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="15">
+        <v>2</v>
+      </c>
+      <c r="P24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="15">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <v>0</v>
+      </c>
+      <c r="U24" s="9">
+        <v>1</v>
+      </c>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2</v>
+      </c>
+      <c r="C25" s="25">
+        <v>54</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <v>2</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <v>0</v>
+      </c>
+      <c r="I25" s="16">
+        <v>2</v>
+      </c>
+      <c r="J25" s="11">
+        <v>1</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+      <c r="L25" s="16">
+        <v>2</v>
+      </c>
+      <c r="M25" s="11">
+        <v>1</v>
+      </c>
+      <c r="N25" s="11">
+        <v>0</v>
+      </c>
+      <c r="O25" s="16">
+        <v>2</v>
+      </c>
+      <c r="P25" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>1</v>
+      </c>
+      <c r="R25" s="16">
+        <v>2</v>
+      </c>
+      <c r="S25" s="11">
+        <v>0</v>
+      </c>
+      <c r="T25" s="5">
+        <v>0</v>
+      </c>
+      <c r="U25" s="12">
+        <v>2</v>
+      </c>
+      <c r="V25" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="W25" s="11">
+        <v>4</v>
+      </c>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+    </row>
+    <row r="27" spans="1:28" ht="48" x14ac:dyDescent="0.2">
+      <c r="C27" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="U27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="R28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="U28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="R29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F30" s="10"/>
+      <c r="W30" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F31" s="10"/>
+      <c r="W31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C158CB6-D266-D744-B859-DD465CD85DD9}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1037,58 +2975,58 @@
         <v>70</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="J1" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="P1" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="S1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="V1" s="8" t="s">
         <v>0</v>
@@ -1112,7 +3050,7 @@
         <v>6</v>
       </c>
       <c r="AC1" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AD1" s="20"/>
       <c r="AG1" s="32"/>
@@ -3451,1939 +5389,6 @@
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F34" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5FF93F-B917-3747-9BBB-00B8CF48955D}">
-  <dimension ref="A1:AB31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="15" width="13.83203125" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="12.5" customWidth="1"/>
-    <col min="22" max="22" width="57.1640625" customWidth="1"/>
-    <col min="23" max="23" width="21.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>2</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="26">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15">
-        <v>2</v>
-      </c>
-      <c r="J2" s="26">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="26">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="15">
-        <v>0</v>
-      </c>
-      <c r="P2" s="26">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>1</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="28">
-        <v>1</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="23">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="15">
-        <v>2</v>
-      </c>
-      <c r="G3" s="13">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="15">
-        <v>2</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>1</v>
-      </c>
-      <c r="R3" s="15">
-        <v>2</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1</v>
-      </c>
-      <c r="T3" s="3">
-        <v>1</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="23">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="15">
-        <v>2</v>
-      </c>
-      <c r="G4" s="13">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="15">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="P4" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="15">
-        <v>1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="3">
-        <v>1</v>
-      </c>
-      <c r="U4" s="9">
-        <v>1</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="23">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
-        <v>2</v>
-      </c>
-      <c r="G5" s="13">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="15">
-        <v>2</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="15">
-        <v>2</v>
-      </c>
-      <c r="P5" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>1</v>
-      </c>
-      <c r="R5" s="15">
-        <v>2</v>
-      </c>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="3">
-        <v>1</v>
-      </c>
-      <c r="U5" s="9">
-        <v>2</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W5" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="23">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M6" s="1">
-        <v>2</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="15">
-        <v>2</v>
-      </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="9">
-        <v>1</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W6" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="23">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="15">
-        <v>2</v>
-      </c>
-      <c r="G7" s="13">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="15">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>0</v>
-      </c>
-      <c r="R7" s="15">
-        <v>2</v>
-      </c>
-      <c r="S7" s="1">
-        <v>1</v>
-      </c>
-      <c r="T7" s="3">
-        <v>1</v>
-      </c>
-      <c r="U7" s="9">
-        <v>2</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W7" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="23">
-        <v>42</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="15">
-        <v>2</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="15">
-        <v>2</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="15">
-        <v>2</v>
-      </c>
-      <c r="P8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>0</v>
-      </c>
-      <c r="R8" s="15">
-        <v>2</v>
-      </c>
-      <c r="S8" s="1">
-        <v>1</v>
-      </c>
-      <c r="T8" s="3">
-        <v>1</v>
-      </c>
-      <c r="U8" s="9">
-        <v>2</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="W8" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="23">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15">
-        <v>2</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="15">
-        <v>1</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="15">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
-      <c r="R9" s="15">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1">
-        <v>1</v>
-      </c>
-      <c r="T9" s="3">
-        <v>0</v>
-      </c>
-      <c r="U9" s="9">
-        <v>1</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W9" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="23">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15">
-        <v>2</v>
-      </c>
-      <c r="G10" s="13">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="15">
-        <v>1</v>
-      </c>
-      <c r="M10" s="1">
-        <v>2</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="15">
-        <v>2</v>
-      </c>
-      <c r="P10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>1</v>
-      </c>
-      <c r="R10" s="15">
-        <v>2</v>
-      </c>
-      <c r="S10" s="1">
-        <v>1</v>
-      </c>
-      <c r="T10" s="3">
-        <v>1</v>
-      </c>
-      <c r="U10" s="9">
-        <v>1</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="W10" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="23">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="15">
-        <v>2</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="15">
-        <v>2</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
-      <c r="L11" s="15">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11" s="15">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="15">
-        <v>2</v>
-      </c>
-      <c r="S11" s="1">
-        <v>0</v>
-      </c>
-      <c r="T11" s="3">
-        <v>0</v>
-      </c>
-      <c r="U11" s="9">
-        <v>2</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W11" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="23">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="15">
-        <v>2</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="15">
-        <v>2</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0</v>
-      </c>
-      <c r="L12" s="15">
-        <v>2</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="15">
-        <v>1</v>
-      </c>
-      <c r="P12" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>0</v>
-      </c>
-      <c r="R12" s="15">
-        <v>1</v>
-      </c>
-      <c r="S12" s="1">
-        <v>1</v>
-      </c>
-      <c r="T12" s="3">
-        <v>0</v>
-      </c>
-      <c r="U12" s="9">
-        <v>1</v>
-      </c>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="23">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="15">
-        <v>2</v>
-      </c>
-      <c r="G13" s="13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="15">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0</v>
-      </c>
-      <c r="L13" s="15">
-        <v>1</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="15">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>0</v>
-      </c>
-      <c r="R13" s="15">
-        <v>1</v>
-      </c>
-      <c r="S13" s="1">
-        <v>1</v>
-      </c>
-      <c r="T13" s="3">
-        <v>0</v>
-      </c>
-      <c r="U13" s="9">
-        <v>1</v>
-      </c>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="23">
-        <v>43</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="15">
-        <v>2</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="15">
-        <v>2</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0</v>
-      </c>
-      <c r="L14" s="15">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14" s="15">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>0</v>
-      </c>
-      <c r="R14" s="15">
-        <v>0</v>
-      </c>
-      <c r="S14" s="1">
-        <v>1</v>
-      </c>
-      <c r="T14" s="3">
-        <v>1</v>
-      </c>
-      <c r="U14" s="9">
-        <v>2</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="W14" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="23">
-        <v>22</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="15">
-        <v>2</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15">
-        <v>2</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="15">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>1</v>
-      </c>
-      <c r="R15" s="15">
-        <v>2</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0</v>
-      </c>
-      <c r="T15" s="3">
-        <v>0</v>
-      </c>
-      <c r="U15" s="9">
-        <v>2</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W15" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="23">
-        <v>58</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="15">
-        <v>2</v>
-      </c>
-      <c r="G16" s="13">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3">
-        <v>1</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="P16" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
-      <c r="R16" s="15">
-        <v>2</v>
-      </c>
-      <c r="S16" s="1">
-        <v>1</v>
-      </c>
-      <c r="T16" s="3">
-        <v>1</v>
-      </c>
-      <c r="U16" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="W16" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="23">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="15">
-        <v>2</v>
-      </c>
-      <c r="G17" s="13">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="15">
-        <v>2</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0</v>
-      </c>
-      <c r="L17" s="15">
-        <v>2</v>
-      </c>
-      <c r="M17" s="1">
-        <v>2</v>
-      </c>
-      <c r="N17" s="1">
-        <v>1</v>
-      </c>
-      <c r="O17" s="15">
-        <v>2</v>
-      </c>
-      <c r="P17" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1</v>
-      </c>
-      <c r="R17" s="15">
-        <v>2</v>
-      </c>
-      <c r="S17" s="1">
-        <v>1</v>
-      </c>
-      <c r="T17" s="3">
-        <v>0</v>
-      </c>
-      <c r="U17" s="9">
-        <v>2</v>
-      </c>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="23">
-        <v>18</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="15">
-        <v>2</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="15">
-        <v>2</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0</v>
-      </c>
-      <c r="L18" s="15">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="O18" s="15">
-        <v>2</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>0</v>
-      </c>
-      <c r="R18" s="15">
-        <v>2</v>
-      </c>
-      <c r="S18" s="1">
-        <v>1</v>
-      </c>
-      <c r="T18" s="3">
-        <v>0</v>
-      </c>
-      <c r="U18" s="9">
-        <v>2</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W18" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="23">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="15">
-        <v>2</v>
-      </c>
-      <c r="G19" s="13">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="I19" s="15">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0</v>
-      </c>
-      <c r="L19" s="15">
-        <v>0</v>
-      </c>
-      <c r="M19" s="1">
-        <v>0</v>
-      </c>
-      <c r="N19" s="1">
-        <v>0</v>
-      </c>
-      <c r="O19" s="15">
-        <v>0</v>
-      </c>
-      <c r="P19" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>0</v>
-      </c>
-      <c r="R19" s="15">
-        <v>2</v>
-      </c>
-      <c r="S19" s="1">
-        <v>1</v>
-      </c>
-      <c r="T19" s="3">
-        <v>0</v>
-      </c>
-      <c r="U19" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>2</v>
-      </c>
-      <c r="C20" s="23">
-        <v>41</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="15">
-        <v>2</v>
-      </c>
-      <c r="G20" s="13">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1">
-        <v>1</v>
-      </c>
-      <c r="I20" s="15">
-        <v>2</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-      <c r="K20" s="3">
-        <v>1</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M20" s="1">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1">
-        <v>0</v>
-      </c>
-      <c r="O20" s="15">
-        <v>0</v>
-      </c>
-      <c r="P20" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>1</v>
-      </c>
-      <c r="R20" s="15">
-        <v>2</v>
-      </c>
-      <c r="S20" s="1">
-        <v>1</v>
-      </c>
-      <c r="T20" s="3">
-        <v>0</v>
-      </c>
-      <c r="U20" s="9">
-        <v>2</v>
-      </c>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>2</v>
-      </c>
-      <c r="C21" s="23">
-        <v>17</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="15">
-        <v>2</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-      <c r="I21" s="15">
-        <v>2</v>
-      </c>
-      <c r="J21" s="1">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0</v>
-      </c>
-      <c r="L21" s="15">
-        <v>2</v>
-      </c>
-      <c r="M21" s="1">
-        <v>2</v>
-      </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21" s="15">
-        <v>2</v>
-      </c>
-      <c r="P21" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>0</v>
-      </c>
-      <c r="R21" s="15">
-        <v>2</v>
-      </c>
-      <c r="S21" s="1">
-        <v>0</v>
-      </c>
-      <c r="T21" s="3">
-        <v>0</v>
-      </c>
-      <c r="U21" s="9">
-        <v>2</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W21" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="23">
-        <v>47</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="15">
-        <v>1</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="15">
-        <v>2</v>
-      </c>
-      <c r="J22" s="1">
-        <v>1</v>
-      </c>
-      <c r="K22" s="3">
-        <v>0</v>
-      </c>
-      <c r="L22" s="15">
-        <v>1</v>
-      </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="15">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>0</v>
-      </c>
-      <c r="R22" s="15">
-        <v>1</v>
-      </c>
-      <c r="S22" s="1">
-        <v>0</v>
-      </c>
-      <c r="T22" s="3">
-        <v>0</v>
-      </c>
-      <c r="U22" s="9">
-        <v>1</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W22" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="23">
-        <v>28</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="15">
-        <v>2</v>
-      </c>
-      <c r="G23" s="13">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="15">
-        <v>2</v>
-      </c>
-      <c r="J23" s="1">
-        <v>1</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M23" s="1">
-        <v>2</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="15">
-        <v>2</v>
-      </c>
-      <c r="P23" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>0</v>
-      </c>
-      <c r="R23" s="15">
-        <v>2</v>
-      </c>
-      <c r="S23" s="1">
-        <v>1</v>
-      </c>
-      <c r="T23" s="3">
-        <v>1</v>
-      </c>
-      <c r="U23" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="W23" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="23">
-        <v>40</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="15">
-        <v>2</v>
-      </c>
-      <c r="G24" s="13">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="15">
-        <v>2</v>
-      </c>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24" s="3">
-        <v>0</v>
-      </c>
-      <c r="L24" s="15">
-        <v>2</v>
-      </c>
-      <c r="M24" s="1">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="15">
-        <v>2</v>
-      </c>
-      <c r="P24" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="3">
-        <v>0</v>
-      </c>
-      <c r="R24" s="15">
-        <v>1</v>
-      </c>
-      <c r="S24" s="1">
-        <v>0</v>
-      </c>
-      <c r="T24" s="3">
-        <v>0</v>
-      </c>
-      <c r="U24" s="9">
-        <v>1</v>
-      </c>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
-        <v>24</v>
-      </c>
-      <c r="B25" s="11">
-        <v>2</v>
-      </c>
-      <c r="C25" s="25">
-        <v>54</v>
-      </c>
-      <c r="D25" s="11">
-        <v>1</v>
-      </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="16">
-        <v>2</v>
-      </c>
-      <c r="G25" s="14">
-        <v>0</v>
-      </c>
-      <c r="H25" s="11">
-        <v>0</v>
-      </c>
-      <c r="I25" s="16">
-        <v>2</v>
-      </c>
-      <c r="J25" s="11">
-        <v>1</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0</v>
-      </c>
-      <c r="L25" s="16">
-        <v>2</v>
-      </c>
-      <c r="M25" s="11">
-        <v>1</v>
-      </c>
-      <c r="N25" s="11">
-        <v>0</v>
-      </c>
-      <c r="O25" s="16">
-        <v>2</v>
-      </c>
-      <c r="P25" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q25" s="5">
-        <v>1</v>
-      </c>
-      <c r="R25" s="16">
-        <v>2</v>
-      </c>
-      <c r="S25" s="11">
-        <v>0</v>
-      </c>
-      <c r="T25" s="5">
-        <v>0</v>
-      </c>
-      <c r="U25" s="12">
-        <v>2</v>
-      </c>
-      <c r="V25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="W25" s="11">
-        <v>4</v>
-      </c>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="F27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="L27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="O27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="R27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="U27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="F28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="R28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="U28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="F29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="L29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="R29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="U29" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="W29" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="F30" s="10"/>
-      <c r="W30" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="F31" s="10"/>
-      <c r="W31" s="1" t="s">
-        <v>92</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5394,7 +5399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30457557-4588-7647-AC7C-B612D7CAAEF7}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
further cleaned analysis notebook
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/empirical_study_DFDs/GitHub_replication_package/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFE2D4A-5BDF-DD44-87B0-DA746A379C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF2A42A-E5D7-5340-8A6C-CA3C0ADC3739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" activeTab="1" xr2:uid="{E68C5B94-9B04-2047-B6F9-6FC8248CDF83}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{E68C5B94-9B04-2047-B6F9-6FC8248CDF83}"/>
   </bookViews>
   <sheets>
     <sheet name="control condition" sheetId="2" r:id="rId1"/>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5FF93F-B917-3747-9BBB-00B8CF48955D}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>78</v>
@@ -1144,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="Q2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" s="15" t="s">
         <v>78</v>
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3" s="15">
         <v>2</v>
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>78</v>
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" s="15">
         <v>2</v>
@@ -1354,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="15">
         <v>2</v>
@@ -1363,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="Q5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5" s="15">
         <v>2</v>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>78</v>
@@ -1427,7 +1427,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="15" t="s">
         <v>78</v>
@@ -1509,7 +1509,7 @@
         <v>2</v>
       </c>
       <c r="Q7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="15">
         <v>2</v>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="15">
         <v>2</v>
@@ -1573,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="N8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" s="15">
         <v>2</v>
@@ -1582,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="15">
         <v>2</v>
@@ -1719,7 +1719,7 @@
         <v>2</v>
       </c>
       <c r="N10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="15">
         <v>2</v>
@@ -1728,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="15">
         <v>2</v>
@@ -1801,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="Q11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="15">
         <v>2</v>
@@ -2089,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="Q15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="15">
         <v>2</v>
@@ -2144,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="15" t="s">
         <v>78</v>
@@ -2153,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="15" t="s">
         <v>78</v>
@@ -2162,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="Q16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="15">
         <v>2</v>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="15">
         <v>2</v>
@@ -2226,7 +2226,7 @@
         <v>2</v>
       </c>
       <c r="N17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O17" s="15">
         <v>2</v>
@@ -2235,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="Q17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" s="15">
         <v>2</v>
@@ -2434,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20" s="15" t="s">
         <v>78</v>
@@ -2452,7 +2452,7 @@
         <v>2</v>
       </c>
       <c r="Q20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R20" s="15">
         <v>2</v>
@@ -2813,7 +2813,7 @@
         <v>2</v>
       </c>
       <c r="Q25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R25" s="16">
         <v>2</v>
@@ -2929,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C158CB6-D266-D744-B859-DD465CD85DD9}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3097,7 +3097,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="15">
         <v>4</v>
@@ -3106,7 +3106,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" s="15" t="s">
         <v>75</v>
@@ -3177,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>75</v>
@@ -3195,7 +3195,7 @@
         <v>2</v>
       </c>
       <c r="Q3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3" s="15" t="s">
         <v>75</v>
@@ -3270,7 +3270,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>75</v>
@@ -3288,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4" s="15" t="s">
         <v>75</v>
@@ -3452,7 +3452,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>75</v>
@@ -3470,7 +3470,7 @@
         <v>2</v>
       </c>
       <c r="Q6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="15" t="s">
         <v>80</v>
@@ -3636,7 +3636,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>75</v>
@@ -3654,7 +3654,7 @@
         <v>2</v>
       </c>
       <c r="Q8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="15" t="s">
         <v>75</v>
@@ -3925,7 +3925,7 @@
         <v>1</v>
       </c>
       <c r="Q11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="15">
         <v>2</v>
@@ -4196,7 +4196,7 @@
         <v>2</v>
       </c>
       <c r="Q14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" s="15">
         <v>2</v>
@@ -4280,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="15" t="s">
         <v>80</v>
@@ -4360,7 +4360,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="15" t="s">
         <v>80</v>
@@ -4378,7 +4378,7 @@
         <v>2</v>
       </c>
       <c r="Q16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="15">
         <v>4</v>
@@ -4451,7 +4451,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="15" t="s">
         <v>76</v>
@@ -4469,7 +4469,7 @@
         <v>2</v>
       </c>
       <c r="Q17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" s="15">
         <v>2</v>
@@ -4629,7 +4629,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="15" t="s">
         <v>75</v>
@@ -4647,7 +4647,7 @@
         <v>2</v>
       </c>
       <c r="Q19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" s="15" t="s">
         <v>82</v>
@@ -4718,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="15">
         <v>3</v>
@@ -4825,7 +4825,7 @@
         <v>1</v>
       </c>
       <c r="Q21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="15">
         <v>2</v>

</xml_diff>

<commit_message>
stucture; anonymized ethical & consent form
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/empirical_study_DFDs/GitHub_replication_package/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF2A42A-E5D7-5340-8A6C-CA3C0ADC3739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C782F1-D37F-EF47-B9E6-6F45C9FAA525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{E68C5B94-9B04-2047-B6F9-6FC8248CDF83}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" activeTab="1" xr2:uid="{E68C5B94-9B04-2047-B6F9-6FC8248CDF83}"/>
   </bookViews>
   <sheets>
     <sheet name="control condition" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="132">
   <si>
     <t xml:space="preserve">How helpful was the provided architectural diagram (Dataflow Diagram) for performing the tasks? </t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>Task6_correctness_of_evidence</t>
+  </si>
+  <si>
+    <t>avergae 4.08</t>
+  </si>
+  <si>
+    <t>average 2,6</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5FF93F-B917-3747-9BBB-00B8CF48955D}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:R25"/>
     </sheetView>
   </sheetViews>
@@ -2929,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C158CB6-D266-D744-B859-DD465CD85DD9}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:R25"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5225,6 +5231,12 @@
       <c r="AJ25" s="1"/>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="V26" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>131</v>
+      </c>
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
@@ -5399,7 +5411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30457557-4588-7647-AC7C-B612D7CAAEF7}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>